<commit_message>
Include the previous year's total budget in the budget summary.
</commit_message>
<xml_diff>
--- a/real_world/brittany_tokai_villas/2017_2018/ReserveFundBudget.xlsx
+++ b/real_world/brittany_tokai_villas/2017_2018/ReserveFundBudget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" state="visible" r:id="rId2"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="145">
   <si>
     <t>ReserveFundBudget</t>
   </si>
@@ -503,7 +503,10 @@
     <t>Reserve fund budget / Total budget</t>
   </si>
   <si>
-    <t>Percentage change in total budget</t>
+    <t>Previous year's total budget</t>
+  </si>
+  <si>
+    <t>Total budget change from previous year (%)</t>
   </si>
   <si>
     <t>Reserve Fund Summary</t>
@@ -947,7 +950,7 @@
   </sheetPr>
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -18473,10 +18476,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -18565,40 +18568,40 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="B13" s="31" t="n">
+      <c r="B13" s="43" t="n">
+        <f aca="false">'Current Financials'!B14</f>
+        <v>907896</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="31" t="n">
         <f aca="false">B11/'Current Financials'!B14-1</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25"/>
-      <c r="B14" s="31"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="45" t="s">
-        <v>135</v>
-      </c>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="25"/>
       <c r="B15" s="31"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="B16" s="26" t="n">
-        <f aca="false">'Planning and Projections'!B18</f>
-        <v>541293</v>
-      </c>
+      <c r="B16" s="31"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B17" s="26" t="n">
-        <f aca="false">'Current Year Planner'!E13</f>
-        <v>1411150</v>
+        <f aca="false">'Planning and Projections'!B18</f>
+        <v>541293</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18606,77 +18609,86 @@
         <v>138</v>
       </c>
       <c r="B18" s="26" t="n">
-        <f aca="false">B16-B17</f>
-        <v>-869857</v>
+        <f aca="false">'Current Year Planner'!E13</f>
+        <v>1411150</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="27" t="n">
-        <f aca="false">(B16-B17)/B17</f>
+      <c r="B19" s="26" t="n">
+        <f aca="false">B17-B18</f>
+        <v>-869857</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="27" t="n">
+        <f aca="false">(B17-B18)/B18</f>
         <v>-0.616417106615172</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
-    </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" s="26" t="n">
-        <f aca="false">'Planning and Projections'!B26</f>
-        <v>381713.538</v>
-      </c>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="s">
         <v>141</v>
       </c>
       <c r="B22" s="26" t="n">
+        <f aca="false">'Planning and Projections'!B26</f>
+        <v>381713.538</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" s="26" t="n">
         <f aca="false">'Current Year Planner'!E19</f>
         <v>871114.374740984</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="26" t="n">
-        <f aca="false">B21-B22</f>
-        <v>-489400.836740984</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="27" t="n">
-        <f aca="false">(B21-B22)/B22</f>
+      <c r="B24" s="26" t="n">
+        <f aca="false">B22-B23</f>
+        <v>-489400.836740984</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="27" t="n">
+        <f aca="false">(B22-B23)/B23</f>
         <v>-0.561810080205027</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
-    </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B26" s="27" t="n">
-        <f aca="false">(B21-B16)/B16</f>
-        <v>-0.294811612195244</v>
-      </c>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="B27" s="46" t="n">
+      <c r="B27" s="27" t="n">
+        <f aca="false">(B22-B17)/B17</f>
+        <v>-0.294811612195244</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="46" t="n">
         <f aca="false">'Planning and Projections'!B27</f>
         <v>5.61509964474758</v>
       </c>

</xml_diff>